<commit_message>
test with data provider refactor
</commit_message>
<xml_diff>
--- a/session_7/data/data.xlsx
+++ b/session_7/data/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/lruiz/Desktop/selenium-testng/session_7/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7998CD00-0B2C-D148-9153-5ADBD8DA625A}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ACA43FB3-CB00-D847-9087-048C7B4AD7D6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16440" xr2:uid="{52D54A86-E619-844E-99E3-BC4802B5C3AA}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>username</t>
   </si>
@@ -55,6 +55,9 @@
   </si>
   <si>
     <t>admin123x</t>
+  </si>
+  <si>
+    <t>123456X</t>
   </si>
 </sst>
 </file>
@@ -416,7 +419,7 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -433,8 +436,8 @@
       <c r="A2" t="s">
         <v>2</v>
       </c>
-      <c r="B2">
-        <v>123456</v>
+      <c r="B2" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>